<commit_message>
(JMT) Added coverage for bl_1s12, 1s16, 1s20, and       1s24
      Modified bl_1s12, init failure due to unknown reasons,
      fixed by rewriting the scenario.
</commit_message>
<xml_diff>
--- a/blocks/bl_1s16/bl_1s16.xlsx
+++ b/blocks/bl_1s16/bl_1s16.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Foretellix\Files\workspace\AV_ValidationVerification\blocks\bl_1s16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E872A4F2-94F8-4502-95D8-FE0E950E5948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3E69A3-930B-4DCE-901E-982B01A2711A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bl_1s6" sheetId="1" r:id="rId1"/>
@@ -58,12 +58,6 @@
     <t>[6..30]m</t>
   </si>
   <si>
-    <t>/pub/home/user4/jmt_workspace</t>
-  </si>
-  <si>
-    <t>/pub/home/user4/workshops/msdl_and_foretify/common/workshop_config.sdl</t>
-  </si>
-  <si>
     <t>npc_speed_gt_dut_start</t>
   </si>
   <si>
@@ -73,13 +67,19 @@
     <t>*bl_1s16</t>
   </si>
   <si>
-    <t>template /pub/home/user4/jmt_workspace/blocks/bl_1s16/bl_1s16.tsdl</t>
-  </si>
-  <si>
     <t>npc_dist_lt_dut_start</t>
   </si>
   <si>
     <t>npc_dist_lt_dut_end</t>
+  </si>
+  <si>
+    <t>template /pub/home/user6/jmt_workspace/blocks/bl_1s16/bl_1s16.tsdl</t>
+  </si>
+  <si>
+    <t>/pub/home/user6/jmt_workspace</t>
+  </si>
+  <si>
+    <t>/pub/home/user6/jmt_workspace/workshop_config.sdl</t>
   </si>
 </sst>
 </file>
@@ -923,7 +923,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +942,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -962,13 +962,13 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -994,7 +994,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -1006,10 +1006,10 @@
         <v>7</v>
       </c>
       <c r="I3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>